<commit_message>
fixed transmission multiplier mispecification
</commit_message>
<xml_diff>
--- a/Tamil_Nadu_Two_Dose/run_dictionary/test_run_2021-06-08.xlsx
+++ b/Tamil_Nadu_Two_Dose/run_dictionary/test_run_2021-06-08.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kpf18\Dropbox (Partners HealthCare)\MPEC Modeling - CEACOV Program\Project 9 - India Vaccination Strategies\9. Python scripts\CEACOV_v10_analysis_scripts\Tamil_Nadu_Two_Dose\run_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45E7D22-2B2A-426D-BACD-A31322278436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17DC5B5A-69E4-434B-A94D-745953C2376F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7428" yWindow="744" windowWidth="12948" windowHeight="10452" xr2:uid="{05E43371-6907-419D-9AA0-0CD1DDD07864}"/>
+    <workbookView xWindow="3804" yWindow="600" windowWidth="18120" windowHeight="10452" xr2:uid="{05E43371-6907-419D-9AA0-0CD1DDD07864}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -544,7 +544,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>run.name</t>
   </si>
@@ -663,10 +663,13 @@
     <t>time.to.coverage</t>
   </si>
   <si>
-    <t>30p_in_12m_12wk_interval</t>
-  </si>
-  <si>
-    <t>30p_in_12m_lumped</t>
+    <t>no_vaccination</t>
+  </si>
+  <si>
+    <t>30p_in_6m_12wk_interval</t>
+  </si>
+  <si>
+    <t>30p_in_6m_lumped</t>
   </si>
 </sst>
 </file>
@@ -787,7 +790,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -800,6 +803,7 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1114,13 +1118,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DEBC09E-C3BF-4DD7-8833-67DCC0A2C60C}">
-  <dimension ref="A1:AM3"/>
+  <dimension ref="A1:AM4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P4" sqref="P4"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1282,7 +1286,7 @@
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2" s="7">
         <v>1000000</v>
@@ -1318,7 +1322,7 @@
         <v>0.3</v>
       </c>
       <c r="M2">
-        <v>360</v>
+        <v>180</v>
       </c>
       <c r="N2">
         <v>1</v>
@@ -1403,7 +1407,7 @@
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B3" s="7">
         <f>B2</f>
@@ -1440,7 +1444,7 @@
         <v>0.3</v>
       </c>
       <c r="M3">
-        <v>360</v>
+        <v>180</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -1520,6 +1524,161 @@
         <v>100</v>
       </c>
       <c r="AM3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="7">
+        <f>B3</f>
+        <v>1000000</v>
+      </c>
+      <c r="C4" s="12">
+        <f>C3</f>
+        <v>0.315</v>
+      </c>
+      <c r="D4" s="12">
+        <f t="shared" ref="D4:AM4" si="0">D3</f>
+        <v>0.62239599999999995</v>
+      </c>
+      <c r="E4" s="12">
+        <f t="shared" si="0"/>
+        <v>0.93359400000000003</v>
+      </c>
+      <c r="F4" s="12">
+        <f t="shared" si="0"/>
+        <v>0.93359400000000003</v>
+      </c>
+      <c r="G4" s="12">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="H4" s="12">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="I4" s="12">
+        <f t="shared" si="0"/>
+        <v>270</v>
+      </c>
+      <c r="J4" s="12">
+        <f t="shared" si="0"/>
+        <v>330</v>
+      </c>
+      <c r="K4" s="12">
+        <f t="shared" si="0"/>
+        <v>0.68</v>
+      </c>
+      <c r="L4" s="12">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>180</v>
+      </c>
+      <c r="N4" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O4" s="12">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="P4" s="12">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="Q4" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R4" s="12">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="S4" s="12">
+        <f t="shared" si="0"/>
+        <v>0.35</v>
+      </c>
+      <c r="T4" s="12">
+        <f t="shared" si="0"/>
+        <v>0.49</v>
+      </c>
+      <c r="U4" s="12">
+        <f t="shared" si="0"/>
+        <v>0.49</v>
+      </c>
+      <c r="V4" s="12">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="W4" s="12">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="X4" s="12">
+        <f t="shared" si="0"/>
+        <v>0.98</v>
+      </c>
+      <c r="Y4" s="12">
+        <f t="shared" si="0"/>
+        <v>0.98</v>
+      </c>
+      <c r="Z4" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AA4" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AB4" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AC4" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AD4" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AE4" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AF4" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AG4" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AH4" s="12">
+        <f t="shared" si="0"/>
+        <v>215.35797619921263</v>
+      </c>
+      <c r="AI4" s="12">
+        <f t="shared" si="0"/>
+        <v>10.769492955526195</v>
+      </c>
+      <c r="AJ4" s="12">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AK4" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AL4" s="12">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="AM4" s="12">
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
     </row>

</xml_diff>